<commit_message>
special proposal creation and reports generation
</commit_message>
<xml_diff>
--- a/caphase3/src/test/java/com/softweb/cure/excels/ProjectOverviewData.xlsx
+++ b/caphase3/src/test/java/com/softweb/cure/excels/ProjectOverviewData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="18030" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14250" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ProjectTitle</t>
   </si>
@@ -67,20 +67,35 @@
     <t>Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. It has survived not only five centuries, but also the leap into electronic typesetting, remaining essentially unchanged. It was popularised in the 1960s with the release of Letraset sheets containing Lorem Ipsum passages, and more recently with desktop publishing software like Aldus PageMaker including versions of Lorem Ipsum.</t>
   </si>
   <si>
-    <t>Special testing proposal</t>
+    <t>ResearchDescription</t>
+  </si>
+  <si>
+    <t>"But I must explain to you how all this mistaken idea of denouncing pleasure and praising pain was born and I will give you a complete account of the system, and expound the actual teachings of the great explorer of the truth, the master-builder of human happiness. No one rejects, dislikes, or avoids pleasure itself, because it is pleasure, but because those who do not know how to pursue pleasure rationally encounter consequences that are extremely painful. Nor again is there anyone who loves or pursues or desires to obtain pain of itself, because it is pain, but because occasionally circumstances occur in which toil and pain can procure him some great pleasure. To take a trivial example, which of us ever undertakes laborious physical exercise, except to obtain some advantage from it? But who has any right to find fault with a man who chooses to enjoy a pleasure that has no annoying consequences, or one who avoids a pain that produces no resultant pleasure?"</t>
+  </si>
+  <si>
+    <t>Spcl Proposal Friday 30 JUNE</t>
+  </si>
+  <si>
+    <t>Friday JUNE Special Proposal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,8 +118,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,9 +439,10 @@
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,13 +470,16 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -480,10 +501,14 @@
       </c>
       <c r="I2" t="s">
         <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
phase 1 completed with reports
</commit_message>
<xml_diff>
--- a/caphase3/src/test/java/com/softweb/cure/excels/ProjectOverviewData.xlsx
+++ b/caphase3/src/test/java/com/softweb/cure/excels/ProjectOverviewData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14250" windowHeight="5340"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14805" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
     <t>Spcl Proposal Friday 30 JUNE</t>
   </si>
   <si>
-    <t>Friday JUNE Special Proposal</t>
+    <t>JULY Special Proposal</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
method for regular proposal started
</commit_message>
<xml_diff>
--- a/caphase3/src/test/java/com/softweb/cure/excels/ProjectOverviewData.xlsx
+++ b/caphase3/src/test/java/com/softweb/cure/excels/ProjectOverviewData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14805" windowHeight="7365"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14250" windowHeight="5640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,10 +73,10 @@
     <t>"But I must explain to you how all this mistaken idea of denouncing pleasure and praising pain was born and I will give you a complete account of the system, and expound the actual teachings of the great explorer of the truth, the master-builder of human happiness. No one rejects, dislikes, or avoids pleasure itself, because it is pleasure, but because those who do not know how to pursue pleasure rationally encounter consequences that are extremely painful. Nor again is there anyone who loves or pursues or desires to obtain pain of itself, because it is pain, but because occasionally circumstances occur in which toil and pain can procure him some great pleasure. To take a trivial example, which of us ever undertakes laborious physical exercise, except to obtain some advantage from it? But who has any right to find fault with a man who chooses to enjoy a pleasure that has no annoying consequences, or one who avoids a pain that produces no resultant pleasure?"</t>
   </si>
   <si>
-    <t>Spcl Proposal Friday 30 JUNE</t>
-  </si>
-  <si>
-    <t>JULY Special Proposal</t>
+    <t>NEW-SPS</t>
+  </si>
+  <si>
+    <t>NEW SPS</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>